<commit_message>
[V1.0 RELEASE]: RELEASE V1.0
</commit_message>
<xml_diff>
--- a/Merge.xlsx
+++ b/Merge.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="109">
   <si>
     <t>ДИТ</t>
   </si>
@@ -316,12 +316,6 @@
     <t>/ca64090f-7d09-4c1a-9fa5-300482dd64b1/Document/Show?letterId=26934b06-f18b-4000-ab27-b2e6f05cab8c&amp;documentId=ddb54622-32d5-4de2-8d2c-37e230e080e8</t>
   </si>
   <si>
-    <t>Счет-фактура №0001008/01004113 от 15.01.20</t>
-  </si>
-  <si>
-    <t>/ca64090f-7d09-4c1a-9fa5-300482dd64b1/Document/Show?letterId=314b2117-31a8-4cec-bd05-8f9e01e6b40c&amp;documentId=defa8496-8193-41c2-915a-70164c66ed37</t>
-  </si>
-  <si>
     <t>363000038606_Соглашение об ЭДО Ростелеком МРФ Волга.pdf</t>
   </si>
   <si>
@@ -347,6 +341,12 @@
   </si>
   <si>
     <t>/ca64090f-7d09-4c1a-9fa5-300482dd64b1/Document/Show?letterId=2da3623b-e2fc-476a-b732-9827bb0365fc&amp;documentId=aa66e86a-a519-4976-bebf-713ae519fb18</t>
+  </si>
+  <si>
+    <t>Акт №2093129026 от 24.01.20</t>
+  </si>
+  <si>
+    <t>/ca64090f-7d09-4c1a-9fa5-300482dd64b1/Document/Show?letterId=61ee49bd-54bf-4c4e-bd0a-21c95cd737eb&amp;documentId=6ec951df-d24b-4478-8155-b0ba0f9b8eaf</t>
   </si>
 </sst>
 </file>
@@ -679,41 +679,41 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>104</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,10 +721,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -732,16 +732,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,13 +749,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -763,41 +763,38 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -819,10 +816,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -833,10 +830,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -847,10 +844,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
@@ -861,10 +858,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -875,10 +872,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
@@ -889,10 +886,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
@@ -903,10 +900,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
@@ -917,10 +914,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>2</v>
@@ -931,10 +928,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
         <v>2</v>
@@ -945,10 +942,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
@@ -959,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
@@ -973,10 +970,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
@@ -987,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
         <v>2</v>
@@ -1001,10 +998,10 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
@@ -1012,44 +1009,44 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,13 +1054,13 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1071,24 +1068,21 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -1099,24 +1093,21 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1127,10 +1118,10 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -1138,16 +1129,16 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D34" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1155,38 +1146,32 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>102</v>
-      </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
         <v>0</v>
@@ -1194,16 +1179,16 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,38 +1196,32 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>8</v>
-      </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>8</v>
-      </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1253,52 +1232,46 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>8</v>
-      </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>83</v>
-      </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1306,10 +1279,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D46" t="s">
         <v>2</v>
@@ -1320,10 +1293,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D47" t="s">
         <v>2</v>
@@ -1334,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -1348,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
@@ -1362,10 +1335,10 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
@@ -1376,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>

</xml_diff>